<commit_message>
ready for a second deploy
</commit_message>
<xml_diff>
--- a/ACTIVOS - EQUIPOS DE COMPUTOS Y OTROS - CAMINOS- PIDICSA  (AG).xlsx
+++ b/ACTIVOS - EQUIPOS DE COMPUTOS Y OTROS - CAMINOS- PIDICSA  (AG).xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Analista de datos\Guías del trabajo\César Bracamonte\Proyecto inventario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6976AD-E260-4D1F-B3E0-D5F820B761F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA74D483-B42B-4152-BCBB-4CCC689B3B70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-48" windowWidth="30936" windowHeight="17496" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Activos fijos" sheetId="1" r:id="rId1"/>
     <sheet name="Base de Datos" sheetId="4" r:id="rId2"/>
-    <sheet name="Facturas de compras de equipo" sheetId="2" r:id="rId3"/>
-    <sheet name="RESUMEN" sheetId="3" r:id="rId4"/>
+    <sheet name="Hoja1" sheetId="5" r:id="rId3"/>
+    <sheet name="Facturas de compras de equipo" sheetId="2" r:id="rId4"/>
+    <sheet name="RESUMEN" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Activos fijos'!$A$2:$N$263</definedName>
@@ -693,8 +694,30 @@
 </comments>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2575" uniqueCount="938">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2831" uniqueCount="938">
   <si>
     <t>p0</t>
   </si>
@@ -4787,7 +4810,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="18">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4803,6 +4826,16 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFF4C7C3"/>
           <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4929,25 +4962,25 @@
   </dxfs>
   <tableStyles count="4">
     <tableStyle name="Activos fijos-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="16"/>
-      <tableStyleElement type="firstRowStripe" dxfId="15"/>
-      <tableStyleElement type="secondRowStripe" dxfId="14"/>
+      <tableStyleElement type="headerRow" dxfId="17"/>
+      <tableStyleElement type="firstRowStripe" dxfId="16"/>
+      <tableStyleElement type="secondRowStripe" dxfId="15"/>
     </tableStyle>
     <tableStyle name="Activos fijos-style 2" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="headerRow" dxfId="13"/>
-      <tableStyleElement type="totalRow" dxfId="12"/>
-      <tableStyleElement type="firstRowStripe" dxfId="11"/>
-      <tableStyleElement type="secondRowStripe" dxfId="10"/>
+      <tableStyleElement type="headerRow" dxfId="14"/>
+      <tableStyleElement type="totalRow" dxfId="13"/>
+      <tableStyleElement type="firstRowStripe" dxfId="12"/>
+      <tableStyleElement type="secondRowStripe" dxfId="11"/>
     </tableStyle>
     <tableStyle name="Facturas de compras de equipo-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
-      <tableStyleElement type="headerRow" dxfId="9"/>
-      <tableStyleElement type="firstRowStripe" dxfId="8"/>
-      <tableStyleElement type="secondRowStripe" dxfId="7"/>
+      <tableStyleElement type="headerRow" dxfId="10"/>
+      <tableStyleElement type="firstRowStripe" dxfId="9"/>
+      <tableStyleElement type="secondRowStripe" dxfId="8"/>
     </tableStyle>
     <tableStyle name="RESUMEN-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF03000000}">
-      <tableStyleElement type="headerRow" dxfId="6"/>
-      <tableStyleElement type="firstRowStripe" dxfId="5"/>
-      <tableStyleElement type="secondRowStripe" dxfId="4"/>
+      <tableStyleElement type="headerRow" dxfId="7"/>
+      <tableStyleElement type="firstRowStripe" dxfId="6"/>
+      <tableStyleElement type="secondRowStripe" dxfId="5"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -5246,9 +5279,9 @@
   </sheetPr>
   <dimension ref="A1:O305"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A235" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3:M260"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.09765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -13660,7 +13693,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F23 C18 E18:E22 G18:G22 G24 F25:F305 G155:G161">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>"CONTAR.SI(F:F,F1)&gt;1"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13681,8 +13714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961BF3DA-A19A-46A2-9EA9-24694047B144}">
   <dimension ref="A1:H256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
-      <selection activeCell="B257" sqref="B257"/>
+    <sheetView tabSelected="1" topLeftCell="A231" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -14134,7 +14167,7 @@
       <c r="F25" s="226"/>
       <c r="G25" s="237"/>
     </row>
-    <row r="26" spans="1:7" ht="112.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>26</v>
       </c>
@@ -18536,13 +18569,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="20" type="noConversion"/>
-  <conditionalFormatting sqref="B1:B21 C16:C20 C22 C153:C157 B23:B256">
-    <cfRule type="expression" dxfId="1" priority="2">
+  <conditionalFormatting sqref="B1:B21 B23:B256 C16:C20 C22 C153:C157">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>"CONTAR.SI(F:F,F1)&gt;1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showDropDown="1" sqref="D1:D256" xr:uid="{01F2A893-0C41-4239-8333-794EA6B61E0F}"/>
@@ -18553,13 +18586,2436 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7A1D41E-EC9A-45C8-8946-B10C8F6A6AA1}">
+  <dimension ref="B1:D256"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B1" s="223" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="str">
+        <f>LEFT(B1,3)</f>
+        <v>AIR</v>
+      </c>
+      <c r="D1" t="str" cm="1">
+        <f t="array" ref="D1:D31">_xlfn.UNIQUE(C1:C256)</f>
+        <v>AIR</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="227" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C65" si="0">LEFT(B2,3)</f>
+        <v>AIR</v>
+      </c>
+      <c r="D2" t="str">
+        <v>ALF</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="223" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>AIR</v>
+      </c>
+      <c r="D3" t="str">
+        <v>ARC</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="227" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>AIR</v>
+      </c>
+      <c r="D4" t="str">
+        <v>BAL</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="223" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>AIR</v>
+      </c>
+      <c r="D5" t="str">
+        <v>BAS</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="227" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>AIR</v>
+      </c>
+      <c r="D6" t="str">
+        <v>BIP</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="223" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>AIR</v>
+      </c>
+      <c r="D7" t="str">
+        <v>BOM</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="227" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>AIR</v>
+      </c>
+      <c r="D8" t="str">
+        <v>CAF</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="223" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>AIR</v>
+      </c>
+      <c r="D9" t="str">
+        <v>CAR</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="227" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>AIR</v>
+      </c>
+      <c r="D10" t="str">
+        <v>DRN</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="223" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>AIR</v>
+      </c>
+      <c r="D11" t="str">
+        <v>DSK</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="227" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>ALF</v>
+      </c>
+      <c r="D12" t="str">
+        <v>ENF</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="232" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>ARC</v>
+      </c>
+      <c r="D13" t="str">
+        <v>GPS</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="234" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>BAL</v>
+      </c>
+      <c r="D14" t="str">
+        <v>IMP</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="232" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>BAL</v>
+      </c>
+      <c r="D15" t="str">
+        <v>LAP</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="234" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>BAL</v>
+      </c>
+      <c r="D16" t="str">
+        <v>MES</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="232" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>BAS</v>
+      </c>
+      <c r="D17" t="str">
+        <v>MIC</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="234" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>BIP</v>
+      </c>
+      <c r="D18" t="str">
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="232" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>BOM</v>
+      </c>
+      <c r="D19" t="str">
+        <v>NEV</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="234" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>CAF</v>
+      </c>
+      <c r="D20" t="str">
+        <v>NIV</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="232" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>CAF</v>
+      </c>
+      <c r="D21" t="str">
+        <v>PAP</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="234" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>CAR</v>
+      </c>
+      <c r="D22" t="str">
+        <v>SSD</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="232" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>DRN</v>
+      </c>
+      <c r="D23" t="str">
+        <v>PRI</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24" s="234" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>DRN</v>
+      </c>
+      <c r="D24" t="str">
+        <v>RAD</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25" s="232" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>DRN</v>
+      </c>
+      <c r="D25" t="str">
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B26" s="234" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>DSK</v>
+      </c>
+      <c r="D26" t="str">
+        <v>SOF</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B27" s="232" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>DSK</v>
+      </c>
+      <c r="D27" t="str">
+        <v>TEV</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B28" s="234" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>DSK</v>
+      </c>
+      <c r="D28" t="str">
+        <v>TOP</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B29" s="232" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>DSK</v>
+      </c>
+      <c r="D29" t="str">
+        <v>TRI</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B30" s="227" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>DSK</v>
+      </c>
+      <c r="D30" t="str">
+        <v>VEN</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B31" s="223" t="s">
+        <v>116</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>DSK</v>
+      </c>
+      <c r="D31" t="str">
+        <v>TEL</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B32" s="227" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>DSK</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33" s="223" t="s">
+        <v>125</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>DSK</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34" s="227" t="s">
+        <v>130</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>DSK</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B35" s="223" t="s">
+        <v>135</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>DSK</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B36" s="227" t="s">
+        <v>140</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>DSK</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B37" s="223" t="s">
+        <v>145</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>DSK</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B38" s="227" t="s">
+        <v>147</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>DSK</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B39" s="223" t="s">
+        <v>152</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>DSK</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B40" s="227" t="s">
+        <v>155</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>DSK</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B41" s="223" t="s">
+        <v>158</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>DSK</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B42" s="227" t="s">
+        <v>163</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>DSK</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B43" s="223" t="s">
+        <v>168</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>DSK</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B44" s="227" t="s">
+        <v>173</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>DSK</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B45" s="223" t="s">
+        <v>178</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>DSK</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B46" s="227" t="s">
+        <v>180</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>DSK</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B47" s="223" t="s">
+        <v>184</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>DSK</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B48" s="227" t="s">
+        <v>186</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v>DSK</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B49" s="223" t="s">
+        <v>190</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>DSK</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B50" s="227" t="s">
+        <v>195</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="0"/>
+        <v>ENF</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B51" s="83" t="s">
+        <v>198</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="0"/>
+        <v>GPS</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B52" s="227" t="s">
+        <v>202</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="0"/>
+        <v>GPS</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B53" s="223" t="s">
+        <v>203</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="0"/>
+        <v>GPS</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B54" s="227" t="s">
+        <v>204</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="0"/>
+        <v>GPS</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B55" s="223" t="s">
+        <v>206</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="0"/>
+        <v>GPS</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B56" s="227" t="s">
+        <v>207</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="0"/>
+        <v>IMP</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B57" s="223" t="s">
+        <v>209</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="0"/>
+        <v>IMP</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B58" s="227" t="s">
+        <v>212</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="0"/>
+        <v>IMP</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B59" s="223" t="s">
+        <v>214</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="0"/>
+        <v>IMP</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B60" s="227" t="s">
+        <v>217</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="0"/>
+        <v>IMP</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B61" s="223" t="s">
+        <v>220</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="0"/>
+        <v>IMP</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B62" s="227" t="s">
+        <v>221</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="0"/>
+        <v>IMP</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B63" s="223" t="s">
+        <v>224</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" si="0"/>
+        <v>IMP</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B64" s="227" t="s">
+        <v>226</v>
+      </c>
+      <c r="C64" t="str">
+        <f t="shared" si="0"/>
+        <v>IMP</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B65" s="223" t="s">
+        <v>937</v>
+      </c>
+      <c r="C65" t="str">
+        <f t="shared" si="0"/>
+        <v>IMP</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B66" s="227" t="s">
+        <v>230</v>
+      </c>
+      <c r="C66" t="str">
+        <f t="shared" ref="C66:C129" si="1">LEFT(B66,3)</f>
+        <v>IMP</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B67" s="223" t="s">
+        <v>232</v>
+      </c>
+      <c r="C67" t="str">
+        <f t="shared" si="1"/>
+        <v>IMP</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B68" s="227" t="s">
+        <v>234</v>
+      </c>
+      <c r="C68" t="str">
+        <f t="shared" si="1"/>
+        <v>IMP</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B69" s="223" t="s">
+        <v>238</v>
+      </c>
+      <c r="C69" t="str">
+        <f t="shared" si="1"/>
+        <v>IMP</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B70" s="227" t="s">
+        <v>241</v>
+      </c>
+      <c r="C70" t="str">
+        <f t="shared" si="1"/>
+        <v>IMP</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B71" s="223" t="s">
+        <v>243</v>
+      </c>
+      <c r="C71" t="str">
+        <f t="shared" si="1"/>
+        <v>IMP</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B72" s="227" t="s">
+        <v>245</v>
+      </c>
+      <c r="C72" t="str">
+        <f t="shared" si="1"/>
+        <v>LAP</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B73" s="223" t="s">
+        <v>250</v>
+      </c>
+      <c r="C73" t="str">
+        <f t="shared" si="1"/>
+        <v>LAP</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B74" s="227" t="s">
+        <v>255</v>
+      </c>
+      <c r="C74" t="str">
+        <f t="shared" si="1"/>
+        <v>LAP</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B75" s="223" t="s">
+        <v>258</v>
+      </c>
+      <c r="C75" t="str">
+        <f t="shared" si="1"/>
+        <v>LAP</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B76" s="227" t="s">
+        <v>262</v>
+      </c>
+      <c r="C76" t="str">
+        <f t="shared" si="1"/>
+        <v>LAP</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B77" s="223" t="s">
+        <v>267</v>
+      </c>
+      <c r="C77" t="str">
+        <f t="shared" si="1"/>
+        <v>LAP</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B78" s="227" t="s">
+        <v>271</v>
+      </c>
+      <c r="C78" t="str">
+        <f t="shared" si="1"/>
+        <v>LAP</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B79" s="223" t="s">
+        <v>273</v>
+      </c>
+      <c r="C79" t="str">
+        <f t="shared" si="1"/>
+        <v>LAP</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B80" s="227" t="s">
+        <v>276</v>
+      </c>
+      <c r="C80" t="str">
+        <f t="shared" si="1"/>
+        <v>LAP</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B81" s="223" t="s">
+        <v>279</v>
+      </c>
+      <c r="C81" t="str">
+        <f t="shared" si="1"/>
+        <v>LAP</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B82" s="227" t="s">
+        <v>282</v>
+      </c>
+      <c r="C82" t="str">
+        <f t="shared" si="1"/>
+        <v>LAP</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B83" s="223" t="s">
+        <v>285</v>
+      </c>
+      <c r="C83" t="str">
+        <f t="shared" si="1"/>
+        <v>LAP</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B84" s="227" t="s">
+        <v>290</v>
+      </c>
+      <c r="C84" t="str">
+        <f t="shared" si="1"/>
+        <v>LAP</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B85" s="223" t="s">
+        <v>292</v>
+      </c>
+      <c r="C85" t="str">
+        <f t="shared" si="1"/>
+        <v>LAP</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B86" s="227" t="s">
+        <v>295</v>
+      </c>
+      <c r="C86" t="str">
+        <f t="shared" si="1"/>
+        <v>LAP</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B87" s="223" t="s">
+        <v>300</v>
+      </c>
+      <c r="C87" t="str">
+        <f t="shared" si="1"/>
+        <v>LAP</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B88" s="227" t="s">
+        <v>302</v>
+      </c>
+      <c r="C88" t="str">
+        <f t="shared" si="1"/>
+        <v>LAP</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B89" s="223" t="s">
+        <v>307</v>
+      </c>
+      <c r="C89" t="str">
+        <f t="shared" si="1"/>
+        <v>LAP</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B90" s="227" t="s">
+        <v>312</v>
+      </c>
+      <c r="C90" t="str">
+        <f t="shared" si="1"/>
+        <v>LAP</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B91" s="223" t="s">
+        <v>316</v>
+      </c>
+      <c r="C91" t="str">
+        <f t="shared" si="1"/>
+        <v>LAP</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B92" s="227" t="s">
+        <v>320</v>
+      </c>
+      <c r="C92" t="str">
+        <f t="shared" si="1"/>
+        <v>LAP</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B93" s="223" t="s">
+        <v>323</v>
+      </c>
+      <c r="C93" t="str">
+        <f t="shared" si="1"/>
+        <v>LAP</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B94" s="227" t="s">
+        <v>326</v>
+      </c>
+      <c r="C94" t="str">
+        <f t="shared" si="1"/>
+        <v>MES</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B95" s="223" t="s">
+        <v>329</v>
+      </c>
+      <c r="C95" t="str">
+        <f t="shared" si="1"/>
+        <v>MES</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B96" s="227" t="s">
+        <v>332</v>
+      </c>
+      <c r="C96" t="str">
+        <f t="shared" si="1"/>
+        <v>MES</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B97" s="223" t="s">
+        <v>334</v>
+      </c>
+      <c r="C97" t="str">
+        <f t="shared" si="1"/>
+        <v>MES</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B98" s="227" t="s">
+        <v>336</v>
+      </c>
+      <c r="C98" t="str">
+        <f t="shared" si="1"/>
+        <v>MES</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B99" s="223" t="s">
+        <v>338</v>
+      </c>
+      <c r="C99" t="str">
+        <f t="shared" si="1"/>
+        <v>MES</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B100" s="227" t="s">
+        <v>340</v>
+      </c>
+      <c r="C100" t="str">
+        <f t="shared" si="1"/>
+        <v>MIC</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B101" s="223" t="s">
+        <v>342</v>
+      </c>
+      <c r="C101" t="str">
+        <f t="shared" si="1"/>
+        <v>MIC</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B102" s="227" t="s">
+        <v>344</v>
+      </c>
+      <c r="C102" t="str">
+        <f t="shared" si="1"/>
+        <v>MIC</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B103" s="223" t="s">
+        <v>347</v>
+      </c>
+      <c r="C103" t="str">
+        <f t="shared" si="1"/>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B104" s="227" t="s">
+        <v>350</v>
+      </c>
+      <c r="C104" t="str">
+        <f t="shared" si="1"/>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B105" s="223" t="s">
+        <v>352</v>
+      </c>
+      <c r="C105" t="str">
+        <f t="shared" si="1"/>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B106" s="227" t="s">
+        <v>355</v>
+      </c>
+      <c r="C106" t="str">
+        <f t="shared" si="1"/>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B107" s="223" t="s">
+        <v>357</v>
+      </c>
+      <c r="C107" t="str">
+        <f t="shared" si="1"/>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B108" s="227" t="s">
+        <v>359</v>
+      </c>
+      <c r="C108" t="str">
+        <f t="shared" si="1"/>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B109" s="223" t="s">
+        <v>361</v>
+      </c>
+      <c r="C109" t="str">
+        <f t="shared" si="1"/>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B110" s="227" t="s">
+        <v>363</v>
+      </c>
+      <c r="C110" t="str">
+        <f t="shared" si="1"/>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="111" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B111" s="223" t="s">
+        <v>366</v>
+      </c>
+      <c r="C111" t="str">
+        <f t="shared" si="1"/>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B112" s="227" t="s">
+        <v>368</v>
+      </c>
+      <c r="C112" t="str">
+        <f t="shared" si="1"/>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B113" s="223" t="s">
+        <v>371</v>
+      </c>
+      <c r="C113" t="str">
+        <f t="shared" si="1"/>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B114" s="227" t="s">
+        <v>373</v>
+      </c>
+      <c r="C114" t="str">
+        <f t="shared" si="1"/>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B115" s="223" t="s">
+        <v>375</v>
+      </c>
+      <c r="C115" t="str">
+        <f t="shared" si="1"/>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B116" s="227" t="s">
+        <v>377</v>
+      </c>
+      <c r="C116" t="str">
+        <f t="shared" si="1"/>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B117" s="223" t="s">
+        <v>379</v>
+      </c>
+      <c r="C117" t="str">
+        <f t="shared" si="1"/>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B118" s="227" t="s">
+        <v>381</v>
+      </c>
+      <c r="C118" t="str">
+        <f t="shared" si="1"/>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B119" s="223" t="s">
+        <v>383</v>
+      </c>
+      <c r="C119" t="str">
+        <f t="shared" si="1"/>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="120" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B120" s="227" t="s">
+        <v>385</v>
+      </c>
+      <c r="C120" t="str">
+        <f t="shared" si="1"/>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B121" s="223" t="s">
+        <v>387</v>
+      </c>
+      <c r="C121" t="str">
+        <f t="shared" si="1"/>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="122" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B122" s="227" t="s">
+        <v>389</v>
+      </c>
+      <c r="C122" t="str">
+        <f t="shared" si="1"/>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B123" s="223" t="s">
+        <v>392</v>
+      </c>
+      <c r="C123" t="str">
+        <f t="shared" si="1"/>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B124" s="227" t="s">
+        <v>394</v>
+      </c>
+      <c r="C124" t="str">
+        <f t="shared" si="1"/>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="125" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B125" s="223" t="s">
+        <v>397</v>
+      </c>
+      <c r="C125" t="str">
+        <f t="shared" si="1"/>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="126" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B126" s="227" t="s">
+        <v>399</v>
+      </c>
+      <c r="C126" t="str">
+        <f t="shared" si="1"/>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="127" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B127" s="223" t="s">
+        <v>400</v>
+      </c>
+      <c r="C127" t="str">
+        <f t="shared" si="1"/>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="128" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B128" s="227" t="s">
+        <v>401</v>
+      </c>
+      <c r="C128" t="str">
+        <f t="shared" si="1"/>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B129" s="223" t="s">
+        <v>404</v>
+      </c>
+      <c r="C129" t="str">
+        <f t="shared" si="1"/>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="130" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B130" s="227" t="s">
+        <v>407</v>
+      </c>
+      <c r="C130" t="str">
+        <f t="shared" ref="C130:C193" si="2">LEFT(B130,3)</f>
+        <v>NEV</v>
+      </c>
+    </row>
+    <row r="131" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B131" s="223" t="s">
+        <v>409</v>
+      </c>
+      <c r="C131" t="str">
+        <f t="shared" si="2"/>
+        <v>NEV</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B132" s="227" t="s">
+        <v>411</v>
+      </c>
+      <c r="C132" t="str">
+        <f t="shared" si="2"/>
+        <v>NEV</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B133" s="223" t="s">
+        <v>414</v>
+      </c>
+      <c r="C133" t="str">
+        <f t="shared" si="2"/>
+        <v>NIV</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B134" s="227" t="s">
+        <v>417</v>
+      </c>
+      <c r="C134" t="str">
+        <f t="shared" si="2"/>
+        <v>NIV</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B135" s="223" t="s">
+        <v>419</v>
+      </c>
+      <c r="C135" t="str">
+        <f t="shared" si="2"/>
+        <v>PAP</v>
+      </c>
+    </row>
+    <row r="136" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B136" s="227" t="s">
+        <v>421</v>
+      </c>
+      <c r="C136" t="str">
+        <f t="shared" si="2"/>
+        <v>SSD</v>
+      </c>
+    </row>
+    <row r="137" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B137" s="223" t="s">
+        <v>424</v>
+      </c>
+      <c r="C137" t="str">
+        <f t="shared" si="2"/>
+        <v>SSD</v>
+      </c>
+    </row>
+    <row r="138" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B138" s="227" t="s">
+        <v>425</v>
+      </c>
+      <c r="C138" t="str">
+        <f t="shared" si="2"/>
+        <v>SSD</v>
+      </c>
+    </row>
+    <row r="139" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B139" s="223" t="s">
+        <v>426</v>
+      </c>
+      <c r="C139" t="str">
+        <f t="shared" si="2"/>
+        <v>SSD</v>
+      </c>
+    </row>
+    <row r="140" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B140" s="83" t="s">
+        <v>427</v>
+      </c>
+      <c r="C140" t="str">
+        <f t="shared" si="2"/>
+        <v>PRI</v>
+      </c>
+    </row>
+    <row r="141" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B141" s="223" t="s">
+        <v>431</v>
+      </c>
+      <c r="C141" t="str">
+        <f t="shared" si="2"/>
+        <v>PRI</v>
+      </c>
+    </row>
+    <row r="142" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B142" s="227" t="s">
+        <v>432</v>
+      </c>
+      <c r="C142" t="str">
+        <f t="shared" si="2"/>
+        <v>PRI</v>
+      </c>
+    </row>
+    <row r="143" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B143" s="83" t="s">
+        <v>434</v>
+      </c>
+      <c r="C143" t="str">
+        <f t="shared" si="2"/>
+        <v>RAD</v>
+      </c>
+    </row>
+    <row r="144" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B144" s="227" t="s">
+        <v>437</v>
+      </c>
+      <c r="C144" t="str">
+        <f t="shared" si="2"/>
+        <v>RAD</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B145" s="223" t="s">
+        <v>438</v>
+      </c>
+      <c r="C145" t="str">
+        <f t="shared" si="2"/>
+        <v>RAD</v>
+      </c>
+    </row>
+    <row r="146" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B146" s="227" t="s">
+        <v>439</v>
+      </c>
+      <c r="C146" t="str">
+        <f t="shared" si="2"/>
+        <v>RAD</v>
+      </c>
+    </row>
+    <row r="147" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B147" s="223" t="s">
+        <v>441</v>
+      </c>
+      <c r="C147" t="str">
+        <f t="shared" si="2"/>
+        <v>RAD</v>
+      </c>
+    </row>
+    <row r="148" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B148" s="227" t="s">
+        <v>442</v>
+      </c>
+      <c r="C148" t="str">
+        <f t="shared" si="2"/>
+        <v>RAD</v>
+      </c>
+    </row>
+    <row r="149" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B149" s="223" t="s">
+        <v>444</v>
+      </c>
+      <c r="C149" t="str">
+        <f t="shared" si="2"/>
+        <v>RAD</v>
+      </c>
+    </row>
+    <row r="150" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B150" s="227" t="s">
+        <v>445</v>
+      </c>
+      <c r="C150" t="str">
+        <f t="shared" si="2"/>
+        <v>RAD</v>
+      </c>
+    </row>
+    <row r="151" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B151" s="223" t="s">
+        <v>447</v>
+      </c>
+      <c r="C151" t="str">
+        <f t="shared" si="2"/>
+        <v>RAD</v>
+      </c>
+    </row>
+    <row r="152" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B152" s="227" t="s">
+        <v>448</v>
+      </c>
+      <c r="C152" t="str">
+        <f t="shared" si="2"/>
+        <v>RAD</v>
+      </c>
+    </row>
+    <row r="153" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B153" s="223" t="s">
+        <v>449</v>
+      </c>
+      <c r="C153" t="str">
+        <f t="shared" si="2"/>
+        <v>RAD</v>
+      </c>
+    </row>
+    <row r="154" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B154" s="227" t="s">
+        <v>450</v>
+      </c>
+      <c r="C154" t="str">
+        <f t="shared" si="2"/>
+        <v>RAD</v>
+      </c>
+    </row>
+    <row r="155" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B155" s="223" t="s">
+        <v>451</v>
+      </c>
+      <c r="C155" t="str">
+        <f t="shared" si="2"/>
+        <v>RAD</v>
+      </c>
+    </row>
+    <row r="156" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B156" s="227" t="s">
+        <v>452</v>
+      </c>
+      <c r="C156" t="str">
+        <f t="shared" si="2"/>
+        <v>RAD</v>
+      </c>
+    </row>
+    <row r="157" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B157" s="232" t="s">
+        <v>453</v>
+      </c>
+      <c r="C157" t="str">
+        <f t="shared" si="2"/>
+        <v>RAD</v>
+      </c>
+    </row>
+    <row r="158" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B158" s="227" t="s">
+        <v>459</v>
+      </c>
+      <c r="C158" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="159" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B159" s="223" t="s">
+        <v>461</v>
+      </c>
+      <c r="C159" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="160" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B160" s="227" t="s">
+        <v>462</v>
+      </c>
+      <c r="C160" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="161" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B161" s="223" t="s">
+        <v>463</v>
+      </c>
+      <c r="C161" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="162" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B162" s="227" t="s">
+        <v>466</v>
+      </c>
+      <c r="C162" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="163" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B163" s="223" t="s">
+        <v>468</v>
+      </c>
+      <c r="C163" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="164" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B164" s="227" t="s">
+        <v>470</v>
+      </c>
+      <c r="C164" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="165" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B165" s="223" t="s">
+        <v>472</v>
+      </c>
+      <c r="C165" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="166" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B166" s="227" t="s">
+        <v>474</v>
+      </c>
+      <c r="C166" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="167" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B167" s="223" t="s">
+        <v>475</v>
+      </c>
+      <c r="C167" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="168" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B168" s="227" t="s">
+        <v>476</v>
+      </c>
+      <c r="C168" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="169" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B169" s="223" t="s">
+        <v>477</v>
+      </c>
+      <c r="C169" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="170" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B170" s="227" t="s">
+        <v>478</v>
+      </c>
+      <c r="C170" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="171" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B171" s="223" t="s">
+        <v>479</v>
+      </c>
+      <c r="C171" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="172" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B172" s="227" t="s">
+        <v>480</v>
+      </c>
+      <c r="C172" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="173" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B173" s="223" t="s">
+        <v>481</v>
+      </c>
+      <c r="C173" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="174" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B174" s="227" t="s">
+        <v>482</v>
+      </c>
+      <c r="C174" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="175" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B175" s="223" t="s">
+        <v>483</v>
+      </c>
+      <c r="C175" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="176" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B176" s="227" t="s">
+        <v>485</v>
+      </c>
+      <c r="C176" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="177" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B177" s="223" t="s">
+        <v>486</v>
+      </c>
+      <c r="C177" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="178" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B178" s="227" t="s">
+        <v>487</v>
+      </c>
+      <c r="C178" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="179" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B179" s="223" t="s">
+        <v>488</v>
+      </c>
+      <c r="C179" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="180" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B180" s="227" t="s">
+        <v>489</v>
+      </c>
+      <c r="C180" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="181" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B181" s="223" t="s">
+        <v>490</v>
+      </c>
+      <c r="C181" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="182" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B182" s="227" t="s">
+        <v>492</v>
+      </c>
+      <c r="C182" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="183" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B183" s="223" t="s">
+        <v>493</v>
+      </c>
+      <c r="C183" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="184" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B184" s="227" t="s">
+        <v>494</v>
+      </c>
+      <c r="C184" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="185" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B185" s="223" t="s">
+        <v>495</v>
+      </c>
+      <c r="C185" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="186" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B186" s="227" t="s">
+        <v>498</v>
+      </c>
+      <c r="C186" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="187" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B187" s="223" t="s">
+        <v>499</v>
+      </c>
+      <c r="C187" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="188" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B188" s="227" t="s">
+        <v>501</v>
+      </c>
+      <c r="C188" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="189" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B189" s="223" t="s">
+        <v>502</v>
+      </c>
+      <c r="C189" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="190" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B190" s="227" t="s">
+        <v>504</v>
+      </c>
+      <c r="C190" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="191" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B191" s="223" t="s">
+        <v>507</v>
+      </c>
+      <c r="C191" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="192" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B192" s="227" t="s">
+        <v>508</v>
+      </c>
+      <c r="C192" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="193" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B193" s="223" t="s">
+        <v>509</v>
+      </c>
+      <c r="C193" t="str">
+        <f t="shared" si="2"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="194" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B194" s="227" t="s">
+        <v>510</v>
+      </c>
+      <c r="C194" t="str">
+        <f t="shared" ref="C194:C257" si="3">LEFT(B194,3)</f>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="195" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B195" s="223" t="s">
+        <v>511</v>
+      </c>
+      <c r="C195" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="196" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B196" s="227" t="s">
+        <v>512</v>
+      </c>
+      <c r="C196" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="197" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B197" s="223" t="s">
+        <v>514</v>
+      </c>
+      <c r="C197" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="198" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B198" s="227" t="s">
+        <v>517</v>
+      </c>
+      <c r="C198" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="199" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B199" s="223" t="s">
+        <v>520</v>
+      </c>
+      <c r="C199" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="200" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B200" s="227" t="s">
+        <v>522</v>
+      </c>
+      <c r="C200" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="201" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B201" s="223" t="s">
+        <v>524</v>
+      </c>
+      <c r="C201" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="202" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B202" s="227" t="s">
+        <v>525</v>
+      </c>
+      <c r="C202" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="203" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B203" s="223" t="s">
+        <v>526</v>
+      </c>
+      <c r="C203" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="204" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B204" s="227" t="s">
+        <v>527</v>
+      </c>
+      <c r="C204" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="205" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B205" s="223" t="s">
+        <v>528</v>
+      </c>
+      <c r="C205" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="206" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B206" s="227" t="s">
+        <v>530</v>
+      </c>
+      <c r="C206" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="207" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B207" s="223" t="s">
+        <v>532</v>
+      </c>
+      <c r="C207" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="208" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B208" s="227" t="s">
+        <v>533</v>
+      </c>
+      <c r="C208" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="209" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B209" s="223" t="s">
+        <v>535</v>
+      </c>
+      <c r="C209" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="210" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B210" s="227" t="s">
+        <v>536</v>
+      </c>
+      <c r="C210" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="211" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B211" s="223" t="s">
+        <v>538</v>
+      </c>
+      <c r="C211" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="212" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B212" s="227" t="s">
+        <v>541</v>
+      </c>
+      <c r="C212" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="213" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B213" s="223" t="s">
+        <v>543</v>
+      </c>
+      <c r="C213" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="214" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B214" s="227" t="s">
+        <v>544</v>
+      </c>
+      <c r="C214" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="215" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B215" s="223" t="s">
+        <v>547</v>
+      </c>
+      <c r="C215" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="216" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B216" s="227" t="s">
+        <v>549</v>
+      </c>
+      <c r="C216" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="217" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B217" s="223" t="s">
+        <v>551</v>
+      </c>
+      <c r="C217" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="218" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B218" s="227" t="s">
+        <v>552</v>
+      </c>
+      <c r="C218" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="219" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B219" s="223" t="s">
+        <v>553</v>
+      </c>
+      <c r="C219" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="220" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B220" s="227" t="s">
+        <v>554</v>
+      </c>
+      <c r="C220" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="221" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B221" s="223" t="s">
+        <v>555</v>
+      </c>
+      <c r="C221" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="222" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B222" s="227" t="s">
+        <v>556</v>
+      </c>
+      <c r="C222" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="223" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B223" s="223" t="s">
+        <v>557</v>
+      </c>
+      <c r="C223" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="224" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B224" s="227" t="s">
+        <v>558</v>
+      </c>
+      <c r="C224" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="225" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B225" s="223" t="s">
+        <v>559</v>
+      </c>
+      <c r="C225" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="226" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B226" s="227" t="s">
+        <v>560</v>
+      </c>
+      <c r="C226" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="227" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B227" s="223" t="s">
+        <v>561</v>
+      </c>
+      <c r="C227" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="228" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B228" s="227" t="s">
+        <v>563</v>
+      </c>
+      <c r="C228" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="229" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B229" s="223" t="s">
+        <v>564</v>
+      </c>
+      <c r="C229" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="230" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B230" s="227" t="s">
+        <v>565</v>
+      </c>
+      <c r="C230" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="231" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B231" s="223" t="s">
+        <v>566</v>
+      </c>
+      <c r="C231" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="232" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B232" s="227" t="s">
+        <v>567</v>
+      </c>
+      <c r="C232" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="233" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B233" s="223" t="s">
+        <v>569</v>
+      </c>
+      <c r="C233" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="234" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B234" s="227" t="s">
+        <v>571</v>
+      </c>
+      <c r="C234" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="235" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B235" s="223" t="s">
+        <v>572</v>
+      </c>
+      <c r="C235" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="236" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B236" s="227" t="s">
+        <v>574</v>
+      </c>
+      <c r="C236" t="str">
+        <f t="shared" si="3"/>
+        <v>SIL</v>
+      </c>
+    </row>
+    <row r="237" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B237" s="223" t="s">
+        <v>575</v>
+      </c>
+      <c r="C237" t="str">
+        <f t="shared" si="3"/>
+        <v>SOF</v>
+      </c>
+    </row>
+    <row r="238" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B238" s="227" t="s">
+        <v>577</v>
+      </c>
+      <c r="C238" t="str">
+        <f t="shared" si="3"/>
+        <v>TEV</v>
+      </c>
+    </row>
+    <row r="239" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B239" s="223" t="s">
+        <v>581</v>
+      </c>
+      <c r="C239" t="str">
+        <f t="shared" si="3"/>
+        <v>TEV</v>
+      </c>
+    </row>
+    <row r="240" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B240" s="227" t="s">
+        <v>583</v>
+      </c>
+      <c r="C240" t="str">
+        <f t="shared" si="3"/>
+        <v>TEV</v>
+      </c>
+    </row>
+    <row r="241" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B241" s="223" t="s">
+        <v>585</v>
+      </c>
+      <c r="C241" t="str">
+        <f t="shared" si="3"/>
+        <v>TEV</v>
+      </c>
+    </row>
+    <row r="242" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B242" s="227" t="s">
+        <v>586</v>
+      </c>
+      <c r="C242" t="str">
+        <f t="shared" si="3"/>
+        <v>TOP</v>
+      </c>
+    </row>
+    <row r="243" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B243" s="223" t="s">
+        <v>590</v>
+      </c>
+      <c r="C243" t="str">
+        <f t="shared" si="3"/>
+        <v>TOP</v>
+      </c>
+    </row>
+    <row r="244" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B244" s="227" t="s">
+        <v>593</v>
+      </c>
+      <c r="C244" t="str">
+        <f t="shared" si="3"/>
+        <v>TOP</v>
+      </c>
+    </row>
+    <row r="245" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B245" s="223" t="s">
+        <v>595</v>
+      </c>
+      <c r="C245" t="str">
+        <f t="shared" si="3"/>
+        <v>TOP</v>
+      </c>
+    </row>
+    <row r="246" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B246" s="227" t="s">
+        <v>598</v>
+      </c>
+      <c r="C246" t="str">
+        <f t="shared" si="3"/>
+        <v>TOP</v>
+      </c>
+    </row>
+    <row r="247" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B247" s="223" t="s">
+        <v>601</v>
+      </c>
+      <c r="C247" t="str">
+        <f t="shared" si="3"/>
+        <v>TOP</v>
+      </c>
+    </row>
+    <row r="248" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B248" s="227" t="s">
+        <v>603</v>
+      </c>
+      <c r="C248" t="str">
+        <f t="shared" si="3"/>
+        <v>TOP</v>
+      </c>
+    </row>
+    <row r="249" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B249" s="223" t="s">
+        <v>606</v>
+      </c>
+      <c r="C249" t="str">
+        <f t="shared" si="3"/>
+        <v>TRI</v>
+      </c>
+    </row>
+    <row r="250" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B250" s="227" t="s">
+        <v>609</v>
+      </c>
+      <c r="C250" t="str">
+        <f t="shared" si="3"/>
+        <v>TRI</v>
+      </c>
+    </row>
+    <row r="251" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B251" s="223" t="s">
+        <v>611</v>
+      </c>
+      <c r="C251" t="str">
+        <f t="shared" si="3"/>
+        <v>TRI</v>
+      </c>
+    </row>
+    <row r="252" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B252" s="227" t="s">
+        <v>612</v>
+      </c>
+      <c r="C252" t="str">
+        <f t="shared" si="3"/>
+        <v>TRI</v>
+      </c>
+    </row>
+    <row r="253" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B253" s="223" t="s">
+        <v>614</v>
+      </c>
+      <c r="C253" t="str">
+        <f t="shared" si="3"/>
+        <v>VEN</v>
+      </c>
+    </row>
+    <row r="254" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B254" s="227" t="s">
+        <v>616</v>
+      </c>
+      <c r="C254" t="str">
+        <f t="shared" si="3"/>
+        <v>VEN</v>
+      </c>
+    </row>
+    <row r="255" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B255" s="223" t="s">
+        <v>618</v>
+      </c>
+      <c r="C255" t="str">
+        <f t="shared" si="3"/>
+        <v>TEL</v>
+      </c>
+    </row>
+    <row r="256" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B256" s="227" t="s">
+        <v>622</v>
+      </c>
+      <c r="C256" t="str">
+        <f t="shared" si="3"/>
+        <v>TEL</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B1:B21 B23:B256">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>"CONTAR.SI(F:F,F1)&gt;1"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.09765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -18946,7 +21402,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:H1000"/>
   <sheetViews>

</xml_diff>